<commit_message>
Caculation of CD0 and e done
</commit_message>
<xml_diff>
--- a/First Measurement Series/Flight20303.xlsx
+++ b/First Measurement Series/Flight20303.xlsx
@@ -188,46 +188,46 @@
     <t>F. used</t>
   </si>
   <si>
+    <t>obs</t>
+  </si>
+  <si>
     <t>[hh:mm:ss]</t>
   </si>
   <si>
     <t>Stationary measurements CL - CD</t>
   </si>
   <si>
-    <t>Xander</t>
-  </si>
-  <si>
     <t>Hans</t>
   </si>
   <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Yaniv</t>
-  </si>
-  <si>
-    <t>Anouk</t>
-  </si>
-  <si>
-    <t>Oussama</t>
-  </si>
-  <si>
-    <t>Floor</t>
-  </si>
-  <si>
-    <t>Alper</t>
-  </si>
-  <si>
-    <t>Yufei</t>
+    <t>Tjipke</t>
+  </si>
+  <si>
+    <t>Maarten</t>
+  </si>
+  <si>
+    <t>Joris</t>
+  </si>
+  <si>
+    <t>Anne-Liza</t>
+  </si>
+  <si>
+    <t>Jordy</t>
+  </si>
+  <si>
+    <t>Willem</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Milan</t>
   </si>
   <si>
     <t>Clean</t>
   </si>
   <si>
     <t>3L</t>
-  </si>
-  <si>
-    <t>cockpit</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -304,14 +304,53 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1028,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,24 +1096,28 @@
         <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>42072</v>
+        <v>42068</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="3">
+        <v>0.3972222222222222</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="3">
+        <v>0.46180555555555558</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1095,10 +1138,10 @@
         <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1106,10 +1149,10 @@
         <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H9" s="2">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1117,10 +1160,10 @@
         <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H10" s="2">
-        <v>98.5</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1128,10 +1171,10 @@
         <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H11" s="2">
-        <v>80</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1139,10 +1182,10 @@
         <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H12" s="2">
-        <v>58.5</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1150,10 +1193,10 @@
         <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H13" s="2">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1161,10 +1204,10 @@
         <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H14" s="2">
-        <v>82.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1172,10 +1215,10 @@
         <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H15" s="2">
-        <v>134.5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1183,10 +1226,10 @@
         <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H16" s="2">
-        <v>109.5</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1194,12 +1237,12 @@
         <v>43</v>
       </c>
       <c r="D18" s="2">
-        <v>2800</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1207,7 +1250,7 @@
         <v>42</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1244,7 +1287,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>12</v>
@@ -1276,32 +1319,32 @@
         <v>1</v>
       </c>
       <c r="B28" s="8">
-        <v>1.042824074074074E-2</v>
+        <v>1.4050925925925927E-2</v>
       </c>
       <c r="C28" s="11">
         <f t="shared" ref="C28:C34" si="0">B28*86400</f>
-        <v>900.99999999999989</v>
+        <v>1214</v>
       </c>
       <c r="D28" s="2">
-        <v>7000</v>
+        <v>5990</v>
       </c>
       <c r="E28" s="2">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F28" s="2">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="G28" s="2">
-        <v>730</v>
+        <v>705</v>
       </c>
       <c r="H28" s="2">
-        <v>790</v>
+        <v>750</v>
       </c>
       <c r="I28" s="2">
-        <v>333</v>
+        <v>403</v>
       </c>
       <c r="J28" s="2">
-        <v>15.2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1309,32 +1352,32 @@
         <v>2</v>
       </c>
       <c r="B29" s="8">
-        <v>1.1736111111111109E-2</v>
+        <v>1.5740740740740743E-2</v>
       </c>
       <c r="C29" s="11">
         <f t="shared" si="0"/>
-        <v>1013.9999999999998</v>
+        <v>1360.0000000000002</v>
       </c>
       <c r="D29" s="2">
-        <v>7010</v>
+        <v>6000</v>
       </c>
       <c r="E29" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F29" s="2">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G29" s="2">
-        <v>620</v>
+        <v>595</v>
       </c>
       <c r="H29" s="2">
-        <v>664</v>
+        <v>647</v>
       </c>
       <c r="I29" s="2">
-        <v>373</v>
+        <v>454</v>
       </c>
       <c r="J29" s="2">
-        <v>13</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1342,32 +1385,32 @@
         <v>3</v>
       </c>
       <c r="B30" s="8">
-        <v>1.3055555555555556E-2</v>
+        <v>1.8518518518518521E-2</v>
       </c>
       <c r="C30" s="11">
         <f t="shared" si="0"/>
-        <v>1128</v>
+        <v>1600.0000000000002</v>
       </c>
       <c r="D30" s="2">
-        <v>7000</v>
+        <v>9000</v>
       </c>
       <c r="E30" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F30" s="2">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="G30" s="2">
-        <v>508</v>
+        <v>470</v>
       </c>
       <c r="H30" s="2">
-        <v>550</v>
+        <v>529</v>
       </c>
       <c r="I30" s="2">
-        <v>405</v>
+        <v>547</v>
       </c>
       <c r="J30" s="2">
-        <v>10.5</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1375,32 +1418,32 @@
         <v>4</v>
       </c>
       <c r="B31" s="8">
-        <v>1.4282407407407409E-2</v>
+        <v>2.074074074074074E-2</v>
       </c>
       <c r="C31" s="11">
         <f t="shared" si="0"/>
-        <v>1234</v>
+        <v>1792</v>
       </c>
       <c r="D31" s="2">
-        <v>7000</v>
+        <v>8990</v>
       </c>
       <c r="E31" s="2">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F31" s="2">
-        <v>4.8</v>
+        <v>5.4</v>
       </c>
       <c r="G31" s="2">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H31" s="2">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I31" s="2">
-        <v>429</v>
+        <v>592</v>
       </c>
       <c r="J31" s="2">
-        <v>9</v>
+        <v>-5.2</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -1408,32 +1451,32 @@
         <v>5</v>
       </c>
       <c r="B32" s="8">
-        <v>1.5601851851851851E-2</v>
+        <v>2.2546296296296297E-2</v>
       </c>
       <c r="C32" s="11">
         <f t="shared" si="0"/>
-        <v>1348</v>
+        <v>1948</v>
       </c>
       <c r="D32" s="2">
-        <v>7000</v>
+        <v>9080</v>
       </c>
       <c r="E32" s="2">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="F32" s="2">
-        <v>6.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G32" s="2">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="H32" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="I32" s="2">
-        <v>453</v>
+        <v>623</v>
       </c>
       <c r="J32" s="2">
-        <v>8</v>
+        <v>-6.5</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -1441,66 +1484,50 @@
         <v>6</v>
       </c>
       <c r="B33" s="8">
-        <v>1.6793981481481483E-2</v>
+        <v>2.4027777777777776E-2</v>
       </c>
       <c r="C33" s="11">
         <f t="shared" si="0"/>
-        <v>1451</v>
+        <v>2076</v>
       </c>
       <c r="D33" s="2">
-        <v>6990</v>
+        <v>9060</v>
       </c>
       <c r="E33" s="2">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F33" s="2">
-        <v>8.6999999999999993</v>
+        <v>11.3</v>
       </c>
       <c r="G33" s="2">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="H33" s="2">
-        <v>435</v>
+        <v>453</v>
       </c>
       <c r="I33" s="2">
-        <v>474</v>
+        <v>651</v>
       </c>
       <c r="J33" s="2">
-        <v>7.2</v>
+        <v>-7.5</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
-      <c r="B34" s="8">
-        <v>1.8449074074074073E-2</v>
-      </c>
+      <c r="B34" s="8"/>
       <c r="C34" s="11">
         <f t="shared" si="0"/>
-        <v>1593.9999999999998</v>
-      </c>
-      <c r="D34" s="2">
-        <v>6990</v>
-      </c>
-      <c r="E34" s="2">
-        <v>118</v>
-      </c>
-      <c r="F34" s="2">
-        <v>10.1</v>
-      </c>
-      <c r="G34" s="2">
-        <v>410</v>
-      </c>
-      <c r="H34" s="2">
-        <v>450</v>
-      </c>
-      <c r="I34" s="2">
-        <v>506</v>
-      </c>
-      <c r="J34" s="2">
-        <v>7</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C35" s="7" t="s">
@@ -1563,7 +1590,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>12</v>
@@ -1604,41 +1631,41 @@
         <v>1</v>
       </c>
       <c r="B43" s="8">
-        <v>2.1111111111111108E-2</v>
+        <v>2.7395833333333338E-2</v>
       </c>
       <c r="C43" s="11">
         <f t="shared" ref="C43:C49" si="1">B43*86400</f>
-        <v>1823.9999999999998</v>
+        <v>2367.0000000000005</v>
       </c>
       <c r="D43" s="2">
-        <v>6920</v>
+        <v>9030</v>
       </c>
       <c r="E43" s="2">
         <v>160</v>
       </c>
       <c r="F43" s="2">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="G43" s="2">
-        <v>-1.5</v>
+        <v>-0.7</v>
       </c>
       <c r="H43" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I43" s="2">
         <v>-1</v>
       </c>
       <c r="J43" s="2">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="K43" s="2">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="L43" s="2">
-        <v>563</v>
+        <v>729</v>
       </c>
       <c r="M43" s="2">
-        <v>8.8000000000000007</v>
+        <v>-6.2</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -1646,41 +1673,41 @@
         <v>2</v>
       </c>
       <c r="B44" s="8">
-        <v>2.2349537037037032E-2</v>
+        <v>2.8483796296296295E-2</v>
       </c>
       <c r="C44" s="11">
         <f t="shared" si="1"/>
-        <v>1930.9999999999995</v>
+        <v>2461</v>
       </c>
       <c r="D44" s="2">
-        <v>7140</v>
+        <v>9250</v>
       </c>
       <c r="E44" s="2">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F44" s="2">
-        <v>6.8</v>
+        <v>6</v>
       </c>
       <c r="G44" s="2">
-        <v>-2.8</v>
+        <v>-1.3</v>
       </c>
       <c r="H44" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I44" s="2">
-        <v>-37</v>
+        <v>-29</v>
       </c>
       <c r="J44" s="2">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="K44" s="2">
-        <v>435</v>
+        <v>451</v>
       </c>
       <c r="L44" s="2">
-        <v>590</v>
+        <v>749</v>
       </c>
       <c r="M44" s="2">
-        <v>7.8</v>
+        <v>-6.8</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -1688,41 +1715,41 @@
         <v>3</v>
       </c>
       <c r="B45" s="8">
-        <v>2.3715277777777776E-2</v>
+        <v>2.9201388888888888E-2</v>
       </c>
       <c r="C45" s="11">
         <f t="shared" si="1"/>
-        <v>2049</v>
+        <v>2523</v>
       </c>
       <c r="D45" s="2">
-        <v>7310</v>
+        <v>9450</v>
       </c>
       <c r="E45" s="2">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="F45" s="2">
-        <v>7.9</v>
+        <v>7</v>
       </c>
       <c r="G45" s="2">
-        <v>-3.5</v>
+        <v>-1.8</v>
       </c>
       <c r="H45" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I45" s="2">
-        <v>-45</v>
+        <v>-35</v>
       </c>
       <c r="J45" s="2">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="K45" s="2">
-        <v>431</v>
+        <v>448</v>
       </c>
       <c r="L45" s="2">
-        <v>614</v>
+        <v>767</v>
       </c>
       <c r="M45" s="2">
-        <v>7</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -1730,41 +1757,41 @@
         <v>4</v>
       </c>
       <c r="B46" s="8">
-        <v>2.4664351851851851E-2</v>
+        <v>3.0034722222222223E-2</v>
       </c>
       <c r="C46" s="11">
         <f t="shared" si="1"/>
-        <v>2131</v>
+        <v>2595</v>
       </c>
       <c r="D46" s="2">
-        <v>7070</v>
+        <v>9670</v>
       </c>
       <c r="E46" s="2">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="F46" s="2">
-        <v>5.9</v>
+        <v>8.6</v>
       </c>
       <c r="G46" s="2">
-        <v>-2.2000000000000002</v>
+        <v>-2.7</v>
       </c>
       <c r="H46" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I46" s="2">
-        <v>-23</v>
+        <v>-51</v>
       </c>
       <c r="J46" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K46" s="2">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="L46" s="2">
-        <v>638</v>
+        <v>783</v>
       </c>
       <c r="M46" s="2">
-        <v>8.5</v>
+        <v>-8.1999999999999993</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
@@ -1772,41 +1799,41 @@
         <v>5</v>
       </c>
       <c r="B47" s="8">
-        <v>2.5555555555555554E-2</v>
+        <v>3.1053240740740742E-2</v>
       </c>
       <c r="C47" s="11">
         <f t="shared" si="1"/>
-        <v>2208</v>
+        <v>2683</v>
       </c>
       <c r="D47" s="2">
-        <v>6520</v>
+        <v>8750</v>
       </c>
       <c r="E47" s="2">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F47" s="2">
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G47" s="2">
-        <v>-0.9</v>
+        <v>-0.2</v>
       </c>
       <c r="H47" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I47" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J47" s="2">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="K47" s="2">
-        <v>447</v>
+        <v>463</v>
       </c>
       <c r="L47" s="2">
-        <v>657</v>
+        <v>806</v>
       </c>
       <c r="M47" s="2">
-        <v>4</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -1814,41 +1841,41 @@
         <v>6</v>
       </c>
       <c r="B48" s="8">
-        <v>2.6481481481481481E-2</v>
+        <v>3.1944444444444449E-2</v>
       </c>
       <c r="C48" s="11">
         <f t="shared" si="1"/>
-        <v>2288</v>
+        <v>2760.0000000000005</v>
       </c>
       <c r="D48" s="2">
-        <v>6130</v>
+        <v>8390</v>
       </c>
       <c r="E48" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F48" s="2">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="G48" s="2">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="H48" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I48" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J48" s="2">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="K48" s="2">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="L48" s="2">
-        <v>672</v>
+        <v>824</v>
       </c>
       <c r="M48" s="2">
-        <v>11.2</v>
+        <v>-4.8</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
@@ -1856,41 +1883,41 @@
         <v>7</v>
       </c>
       <c r="B49" s="8">
-        <v>2.7210648148148147E-2</v>
+        <v>3.27662037037037E-2</v>
       </c>
       <c r="C49" s="11">
         <f t="shared" si="1"/>
-        <v>2351</v>
+        <v>2830.9999999999995</v>
       </c>
       <c r="D49" s="2">
-        <v>5680</v>
+        <v>8020</v>
       </c>
       <c r="E49" s="2">
         <v>188</v>
       </c>
       <c r="F49" s="2">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="G49" s="2">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H49" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I49" s="2">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="J49" s="2">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="K49" s="2">
-        <v>465</v>
+        <v>479</v>
       </c>
       <c r="L49" s="2">
-        <v>693</v>
+        <v>841</v>
       </c>
       <c r="M49" s="2">
-        <v>12</v>
+        <v>-3.8</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
@@ -1908,7 +1935,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
@@ -1916,13 +1943,13 @@
         <v>54</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E55" t="s">
         <v>31</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -1968,7 +1995,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>12</v>
@@ -2009,41 +2036,41 @@
         <v>1</v>
       </c>
       <c r="B59" s="8">
-        <v>2.8807870370370373E-2</v>
+        <v>3.366898148148148E-2</v>
       </c>
       <c r="C59" s="11">
         <f t="shared" ref="C59:C60" si="2">B59*86400</f>
-        <v>2489</v>
+        <v>2909</v>
       </c>
       <c r="D59" s="2">
-        <v>5940</v>
+        <v>8380</v>
       </c>
       <c r="E59" s="2">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F59" s="2">
         <v>4.9000000000000004</v>
       </c>
       <c r="G59" s="2">
-        <v>-1.6</v>
+        <v>-0.7</v>
       </c>
       <c r="H59" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I59" s="2">
         <v>-1</v>
       </c>
       <c r="J59" s="2">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="K59" s="2">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="L59" s="2">
-        <v>723</v>
+        <v>860</v>
       </c>
       <c r="M59" s="2">
-        <v>10.3</v>
+        <v>-5.5</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -2051,41 +2078,41 @@
         <v>2</v>
       </c>
       <c r="B60" s="8">
-        <v>3.0162037037037032E-2</v>
+        <v>3.4571759259259253E-2</v>
       </c>
       <c r="C60" s="11">
         <f t="shared" si="2"/>
-        <v>2605.9999999999995</v>
+        <v>2986.9999999999995</v>
       </c>
       <c r="D60" s="2">
-        <v>5880</v>
+        <v>8480</v>
       </c>
       <c r="E60" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F60" s="2">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="G60" s="2">
-        <v>-2.4</v>
+        <v>-1.5</v>
       </c>
       <c r="H60" s="2">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="I60" s="2">
-        <v>-40</v>
+        <v>-39</v>
       </c>
       <c r="J60" s="2">
         <v>422</v>
       </c>
       <c r="K60" s="2">
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="L60" s="2">
-        <v>753</v>
+        <v>880</v>
       </c>
       <c r="M60" s="2">
-        <v>9.9</v>
+        <v>-5.8</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -2125,19 +2152,19 @@
         <v>34</v>
       </c>
       <c r="D67" s="4">
-        <v>3.1481481481481485E-2</v>
+        <v>3.6805555555555557E-2</v>
       </c>
       <c r="E67" t="s">
         <v>35</v>
       </c>
-      <c r="G67" s="12">
-        <v>3.3333333333333333E-2</v>
+      <c r="G67" s="4">
+        <v>3.9583333333333331E-2</v>
       </c>
       <c r="H67" t="s">
         <v>36</v>
       </c>
       <c r="J67" s="4">
-        <v>3.5300925925925923E-2</v>
+        <v>3.5416666666666666E-2</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -2145,74 +2172,86 @@
         <v>37</v>
       </c>
       <c r="D68" s="4">
-        <v>3.0902777777777779E-2</v>
+        <v>3.6111111111111115E-2</v>
       </c>
       <c r="E68" t="s">
         <v>38</v>
       </c>
-      <c r="G68" s="2"/>
+      <c r="G68" s="4">
+        <v>4.027777777777778E-2</v>
+      </c>
       <c r="H68" t="s">
         <v>39</v>
       </c>
       <c r="J68" s="4">
-        <v>3.740740740740741E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="H3:H4 D8:D16 H8:H16 J67:J68">
-    <cfRule type="containsBlanks" dxfId="16" priority="30">
+  <conditionalFormatting sqref="H3:H4 D8:D16 H8:H16">
+    <cfRule type="containsBlanks" dxfId="18" priority="30">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsBlanks" dxfId="15" priority="25">
+    <cfRule type="containsBlanks" dxfId="17" priority="25">
       <formula>LEN(TRIM(D18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:M49">
-    <cfRule type="containsBlanks" dxfId="14" priority="21">
+    <cfRule type="containsBlanks" dxfId="16" priority="21">
       <formula>LEN(TRIM(D43))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:J34">
-    <cfRule type="containsBlanks" dxfId="13" priority="22">
+    <cfRule type="containsBlanks" dxfId="15" priority="22">
       <formula>LEN(TRIM(D28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsBlanks" dxfId="12" priority="20">
+    <cfRule type="containsBlanks" dxfId="14" priority="20">
       <formula>LEN(TRIM(C54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="containsBlanks" dxfId="11" priority="19">
+    <cfRule type="containsBlanks" dxfId="13" priority="19">
       <formula>LEN(TRIM(C55))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="containsBlanks" dxfId="10" priority="18">
+    <cfRule type="containsBlanks" dxfId="12" priority="18">
       <formula>LEN(TRIM(H55))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59:M60">
-    <cfRule type="containsBlanks" dxfId="9" priority="17">
+    <cfRule type="containsBlanks" dxfId="11" priority="17">
       <formula>LEN(TRIM(D59))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D4">
-    <cfRule type="containsBlanks" dxfId="8" priority="12">
+    <cfRule type="containsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="containsBlanks" dxfId="7" priority="13">
+    <cfRule type="containsBlanks" dxfId="9" priority="13">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67:D68">
-    <cfRule type="containsBlanks" dxfId="6" priority="11">
+    <cfRule type="containsBlanks" dxfId="8" priority="11">
       <formula>LEN(TRIM(D67))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G67:G68">
+    <cfRule type="containsBlanks" dxfId="7" priority="10">
+      <formula>LEN(TRIM(G67))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J67:J68">
+    <cfRule type="containsBlanks" dxfId="6" priority="9">
+      <formula>LEN(TRIM(J67))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:B49">
@@ -2264,55 +2303,55 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
         <f>PFDS!H8</f>
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>PFDS!H9</f>
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>PFDS!H10</f>
-        <v>98.5</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>PFDS!H11</f>
-        <v>80</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>PFDS!H12</f>
-        <v>58.5</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>PFDS!H13</f>
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>PFDS!H14</f>
-        <v>82.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>PFDS!H15</f>
-        <v>134.5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>PFDS!H16</f>
-        <v>109.5</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2323,7 +2362,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>PFDS!D18</f>
-        <v>2800</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2572,249 +2611,249 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <f>PFDS!B28*86400+PFDS!C28</f>
-        <v>1801.9999999999998</v>
+        <v>2428</v>
       </c>
       <c r="B20">
         <f>PFDS!D28</f>
-        <v>7000</v>
+        <v>5990</v>
       </c>
       <c r="C20">
         <f>PFDS!E28</f>
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D20">
         <f>PFDS!F28</f>
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E20">
         <f>PFDS!G28</f>
-        <v>730</v>
+        <v>705</v>
       </c>
       <c r="F20">
         <f>PFDS!H28</f>
-        <v>790</v>
+        <v>750</v>
       </c>
       <c r="G20">
         <f>PFDS!I28</f>
-        <v>333</v>
+        <v>403</v>
       </c>
       <c r="H20">
         <f>PFDS!J28</f>
-        <v>15.2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <f>PFDS!B29*86400+PFDS!C29</f>
-        <v>2027.9999999999995</v>
+        <v>2720.0000000000005</v>
       </c>
       <c r="B21">
         <f>PFDS!D29</f>
-        <v>7010</v>
+        <v>6000</v>
       </c>
       <c r="C21">
         <f>PFDS!E29</f>
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D21">
         <f>PFDS!F29</f>
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E21">
         <f>PFDS!G29</f>
-        <v>620</v>
+        <v>595</v>
       </c>
       <c r="F21">
         <f>PFDS!H29</f>
-        <v>664</v>
+        <v>647</v>
       </c>
       <c r="G21">
         <f>PFDS!I29</f>
-        <v>373</v>
+        <v>454</v>
       </c>
       <c r="H21">
         <f>PFDS!J29</f>
-        <v>13</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <f>PFDS!B30*86400+PFDS!C30</f>
-        <v>2256</v>
+        <v>3200.0000000000005</v>
       </c>
       <c r="B22">
         <f>PFDS!D30</f>
-        <v>7000</v>
+        <v>9000</v>
       </c>
       <c r="C22">
         <f>PFDS!E30</f>
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D22">
         <f>PFDS!F30</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="E22">
         <f>PFDS!G30</f>
-        <v>508</v>
+        <v>470</v>
       </c>
       <c r="F22">
         <f>PFDS!H30</f>
-        <v>550</v>
+        <v>529</v>
       </c>
       <c r="G22">
         <f>PFDS!I30</f>
-        <v>405</v>
+        <v>547</v>
       </c>
       <c r="H22">
         <f>PFDS!J30</f>
-        <v>10.5</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <f>PFDS!B31*86400+PFDS!C31</f>
-        <v>2468</v>
+        <v>3584</v>
       </c>
       <c r="B23">
         <f>PFDS!D31</f>
-        <v>7000</v>
+        <v>8990</v>
       </c>
       <c r="C23">
         <f>PFDS!E31</f>
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D23">
         <f>PFDS!F31</f>
-        <v>4.8</v>
+        <v>5.4</v>
       </c>
       <c r="E23">
         <f>PFDS!G31</f>
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F23">
         <f>PFDS!H31</f>
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G23">
         <f>PFDS!I31</f>
-        <v>429</v>
+        <v>592</v>
       </c>
       <c r="H23">
         <f>PFDS!J31</f>
-        <v>9</v>
+        <v>-5.2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <f>PFDS!B32*86400+PFDS!C32</f>
-        <v>2696</v>
+        <v>3896</v>
       </c>
       <c r="B24">
         <f>PFDS!D32</f>
-        <v>7000</v>
+        <v>9080</v>
       </c>
       <c r="C24">
         <f>PFDS!E32</f>
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="D24">
         <f>PFDS!F32</f>
-        <v>6.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E24">
         <f>PFDS!G32</f>
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="F24">
         <f>PFDS!H32</f>
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="G24">
         <f>PFDS!I32</f>
-        <v>453</v>
+        <v>623</v>
       </c>
       <c r="H24">
         <f>PFDS!J32</f>
-        <v>8</v>
+        <v>-6.5</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <f>PFDS!B33*86400+PFDS!C33</f>
-        <v>2902</v>
+        <v>4152</v>
       </c>
       <c r="B25">
         <f>PFDS!D33</f>
-        <v>6990</v>
+        <v>9060</v>
       </c>
       <c r="C25">
         <f>PFDS!E33</f>
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D25">
         <f>PFDS!F33</f>
-        <v>8.6999999999999993</v>
+        <v>11.3</v>
       </c>
       <c r="E25">
         <f>PFDS!G33</f>
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="F25">
         <f>PFDS!H33</f>
-        <v>435</v>
+        <v>453</v>
       </c>
       <c r="G25">
         <f>PFDS!I33</f>
-        <v>474</v>
+        <v>651</v>
       </c>
       <c r="H25">
         <f>PFDS!J33</f>
-        <v>7.2</v>
+        <v>-7.5</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <f>PFDS!B34*86400+PFDS!C34</f>
-        <v>3187.9999999999995</v>
+        <v>0</v>
       </c>
       <c r="B26">
         <f>PFDS!D34</f>
-        <v>6990</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <f>PFDS!E34</f>
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <f>PFDS!F34</f>
-        <v>10.1</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <f>PFDS!G34</f>
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <f>PFDS!H34</f>
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <f>PFDS!I34</f>
-        <v>506</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <f>PFDS!J34</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <f>PFDS!B43*86400+PFDS!C43</f>
-        <v>3647.9999999999995</v>
+        <v>4734.0000000000009</v>
       </c>
       <c r="B27">
         <f>PFDS!D43</f>
-        <v>6920</v>
+        <v>9030</v>
       </c>
       <c r="C27">
         <f>PFDS!E43</f>
@@ -2822,15 +2861,15 @@
       </c>
       <c r="D27">
         <f>PFDS!F43</f>
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="E27">
         <f>PFDS!G43</f>
-        <v>-1.5</v>
+        <v>-0.7</v>
       </c>
       <c r="F27">
         <f>PFDS!H43</f>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G27">
         <f>PFDS!I43</f>
@@ -2838,263 +2877,263 @@
       </c>
       <c r="H27">
         <f>PFDS!J43</f>
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="I27">
         <f>PFDS!K43</f>
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="J27">
         <f>PFDS!L43</f>
-        <v>563</v>
+        <v>729</v>
       </c>
       <c r="K27">
         <f>PFDS!M43</f>
-        <v>8.8000000000000007</v>
+        <v>-6.2</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <f>PFDS!B44*86400+PFDS!C44</f>
-        <v>3861.9999999999991</v>
+        <v>4922</v>
       </c>
       <c r="B28">
         <f>PFDS!D44</f>
-        <v>7140</v>
+        <v>9250</v>
       </c>
       <c r="C28">
         <f>PFDS!E44</f>
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D28">
         <f>PFDS!F44</f>
-        <v>6.8</v>
+        <v>6</v>
       </c>
       <c r="E28">
         <f>PFDS!G44</f>
-        <v>-2.8</v>
+        <v>-1.3</v>
       </c>
       <c r="F28">
         <f>PFDS!H44</f>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G28">
         <f>PFDS!I44</f>
-        <v>-37</v>
+        <v>-29</v>
       </c>
       <c r="H28">
         <f>PFDS!J44</f>
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="I28">
         <f>PFDS!K44</f>
-        <v>435</v>
+        <v>451</v>
       </c>
       <c r="J28">
         <f>PFDS!L44</f>
-        <v>590</v>
+        <v>749</v>
       </c>
       <c r="K28">
         <f>PFDS!M44</f>
-        <v>7.8</v>
+        <v>-6.8</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <f>PFDS!B45*86400+PFDS!C45</f>
-        <v>4098</v>
+        <v>5046</v>
       </c>
       <c r="B29">
         <f>PFDS!D45</f>
-        <v>7310</v>
+        <v>9450</v>
       </c>
       <c r="C29">
         <f>PFDS!E45</f>
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D29">
         <f>PFDS!F45</f>
-        <v>7.9</v>
+        <v>7</v>
       </c>
       <c r="E29">
         <f>PFDS!G45</f>
-        <v>-3.5</v>
+        <v>-1.8</v>
       </c>
       <c r="F29">
         <f>PFDS!H45</f>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G29">
         <f>PFDS!I45</f>
-        <v>-45</v>
+        <v>-35</v>
       </c>
       <c r="H29">
         <f>PFDS!J45</f>
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="I29">
         <f>PFDS!K45</f>
-        <v>431</v>
+        <v>448</v>
       </c>
       <c r="J29">
         <f>PFDS!L45</f>
-        <v>614</v>
+        <v>767</v>
       </c>
       <c r="K29">
         <f>PFDS!M45</f>
-        <v>7</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <f>PFDS!B46*86400+PFDS!C46</f>
-        <v>4262</v>
+        <v>5190</v>
       </c>
       <c r="B30">
         <f>PFDS!D46</f>
-        <v>7070</v>
+        <v>9670</v>
       </c>
       <c r="C30">
         <f>PFDS!E46</f>
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="D30">
         <f>PFDS!F46</f>
-        <v>5.9</v>
+        <v>8.6</v>
       </c>
       <c r="E30">
         <f>PFDS!G46</f>
-        <v>-2.2000000000000002</v>
+        <v>-2.7</v>
       </c>
       <c r="F30">
         <f>PFDS!H46</f>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G30">
         <f>PFDS!I46</f>
-        <v>-23</v>
+        <v>-51</v>
       </c>
       <c r="H30">
         <f>PFDS!J46</f>
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I30">
         <f>PFDS!K46</f>
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="J30">
         <f>PFDS!L46</f>
-        <v>638</v>
+        <v>783</v>
       </c>
       <c r="K30">
         <f>PFDS!M46</f>
-        <v>8.5</v>
+        <v>-8.1999999999999993</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <f>PFDS!B47*86400+PFDS!C47</f>
-        <v>4416</v>
+        <v>5366</v>
       </c>
       <c r="B31">
         <f>PFDS!D47</f>
-        <v>6520</v>
+        <v>8750</v>
       </c>
       <c r="C31">
         <f>PFDS!E47</f>
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D31">
         <f>PFDS!F47</f>
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E31">
         <f>PFDS!G47</f>
-        <v>-0.9</v>
+        <v>-0.2</v>
       </c>
       <c r="F31">
         <f>PFDS!H47</f>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G31">
         <f>PFDS!I47</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H31">
         <f>PFDS!J47</f>
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="I31">
         <f>PFDS!K47</f>
-        <v>447</v>
+        <v>463</v>
       </c>
       <c r="J31">
         <f>PFDS!L47</f>
-        <v>657</v>
+        <v>806</v>
       </c>
       <c r="K31">
         <f>PFDS!M47</f>
-        <v>4</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <f>PFDS!B48*86400+PFDS!C48</f>
-        <v>4576</v>
+        <v>5520.0000000000009</v>
       </c>
       <c r="B32">
         <f>PFDS!D48</f>
-        <v>6130</v>
+        <v>8390</v>
       </c>
       <c r="C32">
         <f>PFDS!E48</f>
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D32">
         <f>PFDS!F48</f>
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="E32">
         <f>PFDS!G48</f>
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <f>PFDS!H48</f>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G32">
         <f>PFDS!I48</f>
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H32">
         <f>PFDS!J48</f>
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="I32">
         <f>PFDS!K48</f>
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="J32">
         <f>PFDS!L48</f>
-        <v>672</v>
+        <v>824</v>
       </c>
       <c r="K32">
         <f>PFDS!M48</f>
-        <v>11.2</v>
+        <v>-4.8</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <f>PFDS!B59*86400+PFDS!C59</f>
-        <v>4978</v>
+        <v>5818</v>
       </c>
       <c r="B33">
         <f>PFDS!D59</f>
-        <v>5940</v>
+        <v>8380</v>
       </c>
       <c r="C33">
         <f>PFDS!E59</f>
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D33">
         <f>PFDS!F59</f>
@@ -3102,11 +3141,11 @@
       </c>
       <c r="E33">
         <f>PFDS!G59</f>
-        <v>-1.6</v>
+        <v>-0.7</v>
       </c>
       <c r="F33">
         <f>PFDS!H59</f>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G33">
         <f>PFDS!I59</f>
@@ -3114,49 +3153,49 @@
       </c>
       <c r="H33">
         <f>PFDS!J59</f>
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="I33">
         <f>PFDS!K59</f>
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="J33">
         <f>PFDS!L59</f>
-        <v>723</v>
+        <v>860</v>
       </c>
       <c r="K33">
         <f>PFDS!M59</f>
-        <v>10.3</v>
+        <v>-5.5</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <f>PFDS!B60*86400+PFDS!C60</f>
-        <v>5211.9999999999991</v>
+        <v>5973.9999999999991</v>
       </c>
       <c r="B34">
         <f>PFDS!D60</f>
-        <v>5880</v>
+        <v>8480</v>
       </c>
       <c r="C34">
         <f>PFDS!E60</f>
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D34">
         <f>PFDS!F60</f>
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="E34">
         <f>PFDS!G60</f>
-        <v>-2.4</v>
+        <v>-1.5</v>
       </c>
       <c r="F34">
         <f>PFDS!H60</f>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="G34">
         <f>PFDS!I60</f>
-        <v>-40</v>
+        <v>-39</v>
       </c>
       <c r="H34">
         <f>PFDS!J60</f>
@@ -3164,15 +3203,15 @@
       </c>
       <c r="I34">
         <f>PFDS!K60</f>
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="J34">
         <f>PFDS!L60</f>
-        <v>753</v>
+        <v>880</v>
       </c>
       <c r="K34">
         <f>PFDS!M60</f>
-        <v>9.9</v>
+        <v>-5.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>